<commit_message>
Update chart ideas - women
</commit_message>
<xml_diff>
--- a/docs/xlsx/chart_ideas.xlsx
+++ b/docs/xlsx/chart_ideas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\wsw-results\docs\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41B85FC-07B6-4AF5-A461-836BCB8784C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B8F4DE-F0A7-4FD0-9FD1-B68DDAEEBBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E9DC1A38-A0F3-4CE4-A38A-0B8BB0710307}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
   <si>
     <t>Daily Top 10</t>
   </si>
@@ -56,21 +56,12 @@
     <t>Pro Fleet Sailboard</t>
   </si>
   <si>
-    <t>First Time Kite Fleet</t>
-  </si>
-  <si>
     <t>Kite Fleet</t>
   </si>
   <si>
-    <t>First Time Wing Fleet</t>
-  </si>
-  <si>
     <t>Wing Fleet</t>
   </si>
   <si>
-    <t>First Time Boat Fleet</t>
-  </si>
-  <si>
     <t>Boat Fleet</t>
   </si>
   <si>
@@ -104,9 +95,6 @@
     <t>All runs for top 10 pro fleet</t>
   </si>
   <si>
-    <t>Women's Fleet</t>
-  </si>
-  <si>
     <t>All runs for top 10 kites</t>
   </si>
   <si>
@@ -128,21 +116,9 @@
     <t># reports</t>
   </si>
   <si>
-    <t>All runs for top 10 first time boats</t>
-  </si>
-  <si>
-    <t>All runs for top 10 first time wings</t>
-  </si>
-  <si>
-    <t>All runs for top 10 first time kites</t>
-  </si>
-  <si>
     <t>All runs for top 10 women</t>
   </si>
   <si>
-    <t>All runs for top 10 first time sailboards</t>
-  </si>
-  <si>
     <t>All runs for top 10 youths</t>
   </si>
   <si>
@@ -179,9 +155,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Does not correspond to daily report - maybe consider a config change?</t>
-  </si>
-  <si>
     <t>No daily report but maybe it should be added?</t>
   </si>
   <si>
@@ -204,6 +177,15 @@
   </si>
   <si>
     <t>Different colour for each fleet / status - 10 in total</t>
+  </si>
+  <si>
+    <t>All runs for top 10 first timers</t>
+  </si>
+  <si>
+    <t>Women's Fleet Sailboard</t>
+  </si>
+  <si>
+    <t>Women</t>
   </si>
 </sst>
 </file>
@@ -289,13 +271,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>295276</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>81304</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -712,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B72457B-FC8A-4719-B936-3E07B620DD98}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,22 +712,22 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -759,13 +741,13 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -776,16 +758,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -799,13 +781,13 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -819,13 +801,13 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -839,13 +821,13 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -859,13 +841,13 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -879,61 +861,38 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -942,18 +901,18 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -962,18 +921,18 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -982,81 +941,84 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" t="s">
         <v>25</v>
-      </c>
-      <c r="E14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3">
-        <v>10</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -1065,116 +1027,96 @@
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1">
-        <v>10</v>
-      </c>
-      <c r="D21" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="B24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>50</v>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F25" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>